<commit_message>
Modificaciones y nuevos ejercicios
</commit_message>
<xml_diff>
--- a/SolucionesBBDD/plantilla-respuestas.xlsx
+++ b/SolucionesBBDD/plantilla-respuestas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgr/git/EjerciciosDNS/SolucionesBBDD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735D6E2C-D5BC-F54F-AA38-4F622F98CE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2D85E7-F136-0D4D-8E04-182C7AD47738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31060" yWindow="700" windowWidth="36800" windowHeight="20680" xr2:uid="{20D91826-AEEB-6446-94AD-D0E852347CD3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="13">
   <si>
     <t>Sender</t>
   </si>
@@ -76,32 +76,15 @@
   <si>
     <t>Aaddr</t>
   </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>correo.uah.es</t>
-  </si>
-  <si>
-    <t>Ipcorreo</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,16 +107,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -468,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA43AE1A-8D47-3747-BCFD-086E01557220}">
   <dimension ref="A1:BH17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AY3" sqref="AY3:BH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,26 +643,26 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="J2" t="s">
         <v>2</v>
@@ -883,26 +863,26 @@
       <c r="N3">
         <v>2</v>
       </c>
-      <c r="O3">
-        <v>5</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>14</v>
+      <c r="O3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" t="s">
+        <v>2</v>
       </c>
       <c r="U3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="V3" t="s">
         <v>2</v>
@@ -1181,35 +1161,35 @@
       <c r="AX4">
         <v>5</v>
       </c>
-      <c r="AY4">
-        <v>2</v>
-      </c>
-      <c r="AZ4">
-        <v>1</v>
-      </c>
-      <c r="BA4">
-        <v>1</v>
-      </c>
-      <c r="BB4">
-        <v>0</v>
-      </c>
-      <c r="BC4">
-        <v>1</v>
+      <c r="AY4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>2</v>
       </c>
       <c r="BD4" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="BE4" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="BF4" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="BG4" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="BH4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.2">
@@ -1257,35 +1237,35 @@
       <c r="N5">
         <v>2</v>
       </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
+      <c r="O5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" t="s">
+        <v>2</v>
       </c>
       <c r="T5" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="U5" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="V5" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="W5" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="X5" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="Y5">
         <f t="shared" si="2"/>
@@ -3644,10 +3624,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="www.uah.es" xr:uid="{FCFF5DAE-A486-2345-908F-9F38C5A205C7}"/>
-    <hyperlink ref="T3" r:id="rId2" display="www.uah.es" xr:uid="{54DCA290-EC02-9A49-8B41-43AD097C4610}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>